<commit_message>
Estructura inicial del proyecto Ruleta de la Vida
</commit_message>
<xml_diff>
--- a/Ruleta de la vida.xlsx
+++ b/Ruleta de la vida.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jake0\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DANIELA\Downloads\Ciencia-de-Datos-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D47A11-F4C7-4DA1-A690-90E9B31746B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6942742A-C12F-4A1A-A98F-23306A8D7323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6984B28C-8822-4239-A549-835564DAEF38}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6984B28C-8822-4239-A549-835564DAEF38}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -138,7 +138,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,7 +165,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,6 +175,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEAA7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -191,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -207,571 +219,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="112">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE389"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1CC65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE389"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1CC65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1CC65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE389"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1CC65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE389"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE389"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1CC65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1CC65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE389"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1CC65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE389"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF1CC65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE389"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1275,6 +729,566 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE389"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1CC65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE389"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1CC65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1CC65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE389"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1CC65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE389"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE389"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1CC65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1CC65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE389"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1CC65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE389"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1CC65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE389"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3104,88 +3118,88 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5188A35E-5C05-4879-AE81-98DFAE29A429}" name="Tabla2" displayName="Tabla2" ref="A2:B5" totalsRowShown="0" headerRowDxfId="111" dataDxfId="110">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5188A35E-5C05-4879-AE81-98DFAE29A429}" name="Tabla2" displayName="Tabla2" ref="A2:B5" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A2:B5" xr:uid="{5188A35E-5C05-4879-AE81-98DFAE29A429}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{D217CECA-3EFB-41B5-B6F0-53A6D1DD85E0}" name="1. Salud y bienestar:" dataDxfId="109"/>
-    <tableColumn id="2" xr3:uid="{0C760BB8-FFFD-40DB-A098-CADCDCD0BFD9}" name="Calificación" dataDxfId="108"/>
+    <tableColumn id="1" xr3:uid="{D217CECA-3EFB-41B5-B6F0-53A6D1DD85E0}" name="1. Salud y bienestar:" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{0C760BB8-FFFD-40DB-A098-CADCDCD0BFD9}" name="Calificación" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CF4F622E-09A5-45D7-A412-EAE909C9391F}" name="Tabla4" displayName="Tabla4" ref="A7:B9" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CF4F622E-09A5-45D7-A412-EAE909C9391F}" name="Tabla4" displayName="Tabla4" ref="A7:B9" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A7:B9" xr:uid="{CF4F622E-09A5-45D7-A412-EAE909C9391F}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{CF0B79E5-9FC6-4045-B032-B377ADD18E77}" name="2. Relaciones:" dataDxfId="105"/>
-    <tableColumn id="2" xr3:uid="{27495AB0-95BA-4AC9-A632-307F1438209B}" name="Calificación" dataDxfId="104"/>
+    <tableColumn id="1" xr3:uid="{CF0B79E5-9FC6-4045-B032-B377ADD18E77}" name="2. Relaciones:" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{27495AB0-95BA-4AC9-A632-307F1438209B}" name="Calificación" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DEA69EDC-56F5-40C8-9BD0-BEEA46F6595A}" name="Tabla5" displayName="Tabla5" ref="A11:B14" totalsRowShown="0" headerRowDxfId="103" dataDxfId="102">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DEA69EDC-56F5-40C8-9BD0-BEEA46F6595A}" name="Tabla5" displayName="Tabla5" ref="A11:B14" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A11:B14" xr:uid="{DEA69EDC-56F5-40C8-9BD0-BEEA46F6595A}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{AF95281E-AC78-4177-82BA-26214C10E384}" name="3. Carrera y propósito:" dataDxfId="101"/>
-    <tableColumn id="2" xr3:uid="{175AD775-80AD-4717-ADBF-9B6AF0DFE9E0}" name="Calificación" dataDxfId="100"/>
+    <tableColumn id="1" xr3:uid="{AF95281E-AC78-4177-82BA-26214C10E384}" name="3. Carrera y propósito:" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{175AD775-80AD-4717-ADBF-9B6AF0DFE9E0}" name="Calificación" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7B49A688-7883-41E5-B4A5-F0511F56559F}" name="Tabla6" displayName="Tabla6" ref="A16:B19" totalsRowShown="0" headerRowDxfId="99" dataDxfId="98">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7B49A688-7883-41E5-B4A5-F0511F56559F}" name="Tabla6" displayName="Tabla6" ref="A16:B19" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A16:B19" xr:uid="{7B49A688-7883-41E5-B4A5-F0511F56559F}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{7CE2BDAE-71D7-4A9E-9131-CF525D9FDF92}" name="4. Finanzas:" dataDxfId="97"/>
-    <tableColumn id="2" xr3:uid="{FFD8FD1A-0304-48C2-A633-85EEB9B82360}" name="Calificación" dataDxfId="96"/>
+    <tableColumn id="1" xr3:uid="{7CE2BDAE-71D7-4A9E-9131-CF525D9FDF92}" name="4. Finanzas:" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{FFD8FD1A-0304-48C2-A633-85EEB9B82360}" name="Calificación" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{638BA9EA-3861-4FFF-B9CD-1A6D9A304D6E}" name="Tabla7" displayName="Tabla7" ref="A21:B24" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{638BA9EA-3861-4FFF-B9CD-1A6D9A304D6E}" name="Tabla7" displayName="Tabla7" ref="A21:B24" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A21:B24" xr:uid="{638BA9EA-3861-4FFF-B9CD-1A6D9A304D6E}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{70B4A0C1-753F-4DBE-A5CE-D3A2F05D21C0}" name="5. Desarrollo personal y crecimiento:" dataDxfId="93"/>
-    <tableColumn id="2" xr3:uid="{E00D557E-BF20-4AC5-BCCD-FCD3D9F2AF16}" name="Calificación" dataDxfId="92"/>
+    <tableColumn id="1" xr3:uid="{70B4A0C1-753F-4DBE-A5CE-D3A2F05D21C0}" name="5. Desarrollo personal y crecimiento:" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{E00D557E-BF20-4AC5-BCCD-FCD3D9F2AF16}" name="Calificación" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{3CF7AF47-953D-4738-99AC-5EA8F3F99058}" name="Tabla8" displayName="Tabla8" ref="A26:B29" totalsRowShown="0" headerRowDxfId="91" dataDxfId="90">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{3CF7AF47-953D-4738-99AC-5EA8F3F99058}" name="Tabla8" displayName="Tabla8" ref="A26:B29" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A26:B29" xr:uid="{3CF7AF47-953D-4738-99AC-5EA8F3F99058}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3FA219AC-49A2-4A50-AAD9-DD956281B6A3}" name="6. Diversión y ocio:" dataDxfId="89"/>
-    <tableColumn id="2" xr3:uid="{E2C6FA95-321E-41D4-9EEE-8329F8B102B9}" name="Calificación" dataDxfId="88"/>
+    <tableColumn id="1" xr3:uid="{3FA219AC-49A2-4A50-AAD9-DD956281B6A3}" name="6. Diversión y ocio:" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{E2C6FA95-321E-41D4-9EEE-8329F8B102B9}" name="Calificación" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{CD95914E-0441-4A6E-A6B5-4AA7FED13B98}" name="Tabla9" displayName="Tabla9" ref="A31:B34" totalsRowShown="0" headerRowDxfId="87" dataDxfId="86">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{CD95914E-0441-4A6E-A6B5-4AA7FED13B98}" name="Tabla9" displayName="Tabla9" ref="A31:B34" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A31:B34" xr:uid="{CD95914E-0441-4A6E-A6B5-4AA7FED13B98}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{0DB46D41-3F5D-4A4F-819A-7BCC04480389}" name="7. Espiritualidad:" dataDxfId="85"/>
-    <tableColumn id="2" xr3:uid="{AF3EECFA-4DC9-4FA3-BC4D-2F368878581A}" name="Calificación" dataDxfId="84"/>
+    <tableColumn id="1" xr3:uid="{0DB46D41-3F5D-4A4F-819A-7BCC04480389}" name="7. Espiritualidad:" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{AF3EECFA-4DC9-4FA3-BC4D-2F368878581A}" name="Calificación" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{FB8B69F6-D543-471B-964B-446DB0452D59}" name="Tabla10" displayName="Tabla10" ref="A36:B39" totalsRowShown="0" headerRowDxfId="83" dataDxfId="82">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{FB8B69F6-D543-471B-964B-446DB0452D59}" name="Tabla10" displayName="Tabla10" ref="A36:B39" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A36:B39" xr:uid="{FB8B69F6-D543-471B-964B-446DB0452D59}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{0219640A-C97E-4EA1-A77D-970C14BBA328}" name="8. Entorno físico y hogar:" dataDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{673AEF35-49A6-4DBE-8308-5A4189DB8CEF}" name="Calificación" dataDxfId="80"/>
+    <tableColumn id="1" xr3:uid="{0219640A-C97E-4EA1-A77D-970C14BBA328}" name="8. Entorno físico y hogar:" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{673AEF35-49A6-4DBE-8308-5A4189DB8CEF}" name="Calificación" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium24" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3511,21 +3525,21 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="88.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="88.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -3537,8 +3551,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:4" ht="15">
+      <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="5">
@@ -3549,7 +3563,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -3561,8 +3575,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:4" ht="15">
+      <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="4">
@@ -3573,14 +3587,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="D6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15">
       <c r="A7" s="3" t="s">
         <v>25</v>
       </c>
@@ -3591,7 +3605,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="15">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
@@ -3603,7 +3617,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
@@ -3615,7 +3629,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="15">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="2"/>
@@ -3623,7 +3637,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15">
       <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
@@ -3634,8 +3648,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:4" ht="15">
+      <c r="A12" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4">
@@ -3643,7 +3657,7 @@
       </c>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="15">
       <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
@@ -3652,8 +3666,8 @@
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:4" ht="15">
+      <c r="A14" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="4">
@@ -3661,11 +3675,11 @@
       </c>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="15">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="15">
       <c r="A16" s="3" t="s">
         <v>27</v>
       </c>
@@ -3673,7 +3687,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="15">
       <c r="A17" s="3" t="s">
         <v>8</v>
       </c>
@@ -3682,7 +3696,7 @@
       </c>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15">
       <c r="A18" s="3" t="s">
         <v>9</v>
       </c>
@@ -3691,7 +3705,7 @@
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="15">
       <c r="A19" s="3" t="s">
         <v>10</v>
       </c>
@@ -3700,11 +3714,11 @@
       </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="15">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="15">
       <c r="A21" s="3" t="s">
         <v>28</v>
       </c>
@@ -3712,7 +3726,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="15">
       <c r="A22" s="3" t="s">
         <v>11</v>
       </c>
@@ -3721,7 +3735,7 @@
       </c>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="15">
       <c r="A23" s="3" t="s">
         <v>12</v>
       </c>
@@ -3730,7 +3744,7 @@
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="15">
       <c r="A24" s="3" t="s">
         <v>13</v>
       </c>
@@ -3739,11 +3753,11 @@
       </c>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="15">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
     </row>
-    <row r="26" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="15">
       <c r="A26" s="3" t="s">
         <v>29</v>
       </c>
@@ -3751,7 +3765,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="15">
       <c r="A27" s="3" t="s">
         <v>14</v>
       </c>
@@ -3760,7 +3774,7 @@
       </c>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="15">
       <c r="A28" s="3" t="s">
         <v>15</v>
       </c>
@@ -3769,7 +3783,7 @@
       </c>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="15">
       <c r="A29" s="3" t="s">
         <v>22</v>
       </c>
@@ -3778,11 +3792,11 @@
       </c>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="15">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="15">
       <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
@@ -3790,7 +3804,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="15">
       <c r="A32" s="3" t="s">
         <v>16</v>
       </c>
@@ -3799,7 +3813,7 @@
       </c>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="15">
       <c r="A33" s="3" t="s">
         <v>17</v>
       </c>
@@ -3808,7 +3822,7 @@
       </c>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="15">
       <c r="A34" s="3" t="s">
         <v>18</v>
       </c>
@@ -3817,11 +3831,11 @@
       </c>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="15">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
     </row>
-    <row r="36" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="15">
       <c r="A36" s="3" t="s">
         <v>31</v>
       </c>
@@ -3829,7 +3843,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="15">
       <c r="A37" s="3" t="s">
         <v>19</v>
       </c>
@@ -3838,7 +3852,7 @@
       </c>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="15">
       <c r="A38" s="3" t="s">
         <v>20</v>
       </c>
@@ -3847,7 +3861,7 @@
       </c>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="15">
       <c r="A39" s="3" t="s">
         <v>21</v>
       </c>
@@ -3859,258 +3873,258 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B3:C5">
-    <cfRule type="containsText" dxfId="79" priority="89" operator="containsText" text="2">
+    <cfRule type="containsText" dxfId="111" priority="89" operator="containsText" text="2">
       <formula>NOT(ISERROR(SEARCH("2",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="88" operator="containsText" text="3">
+    <cfRule type="containsText" dxfId="110" priority="88" operator="containsText" text="3">
       <formula>NOT(ISERROR(SEARCH("3",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="87" operator="containsText" text="4">
+    <cfRule type="containsText" dxfId="109" priority="87" operator="containsText" text="4">
       <formula>NOT(ISERROR(SEARCH("4",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="86" operator="containsText" text="5">
+    <cfRule type="containsText" dxfId="108" priority="86" operator="containsText" text="5">
       <formula>NOT(ISERROR(SEARCH("5",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="85" operator="containsText" text="6">
+    <cfRule type="containsText" dxfId="107" priority="85" operator="containsText" text="6">
       <formula>NOT(ISERROR(SEARCH("6",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="84" operator="containsText" text="7">
+    <cfRule type="containsText" dxfId="106" priority="84" operator="containsText" text="7">
       <formula>NOT(ISERROR(SEARCH("7",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="83" operator="containsText" text="8">
+    <cfRule type="containsText" dxfId="105" priority="83" operator="containsText" text="8">
       <formula>NOT(ISERROR(SEARCH("8",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="82" operator="containsText" text="9">
+    <cfRule type="containsText" dxfId="104" priority="82" operator="containsText" text="9">
       <formula>NOT(ISERROR(SEARCH("9",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="81" operator="containsText" text="10">
+    <cfRule type="containsText" dxfId="103" priority="81" operator="containsText" text="10">
       <formula>NOT(ISERROR(SEARCH("10",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="90" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="102" priority="90" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:C9">
-    <cfRule type="containsText" dxfId="69" priority="68" operator="containsText" text="3">
+    <cfRule type="containsText" dxfId="101" priority="68" operator="containsText" text="3">
       <formula>NOT(ISERROR(SEARCH("3",B8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="70" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="100" priority="70" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",B8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="69" operator="containsText" text="2">
+    <cfRule type="containsText" dxfId="99" priority="69" operator="containsText" text="2">
       <formula>NOT(ISERROR(SEARCH("2",B8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="67" operator="containsText" text="4">
+    <cfRule type="containsText" dxfId="98" priority="67" operator="containsText" text="4">
       <formula>NOT(ISERROR(SEARCH("4",B8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="66" operator="containsText" text="5">
+    <cfRule type="containsText" dxfId="97" priority="66" operator="containsText" text="5">
       <formula>NOT(ISERROR(SEARCH("5",B8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="6">
+    <cfRule type="containsText" dxfId="96" priority="65" operator="containsText" text="6">
       <formula>NOT(ISERROR(SEARCH("6",B8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="64" operator="containsText" text="7">
+    <cfRule type="containsText" dxfId="95" priority="64" operator="containsText" text="7">
       <formula>NOT(ISERROR(SEARCH("7",B8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="63" operator="containsText" text="8">
+    <cfRule type="containsText" dxfId="94" priority="63" operator="containsText" text="8">
       <formula>NOT(ISERROR(SEARCH("8",B8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="62" operator="containsText" text="9">
+    <cfRule type="containsText" dxfId="93" priority="62" operator="containsText" text="9">
       <formula>NOT(ISERROR(SEARCH("9",B8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="61" operator="containsText" text="10">
+    <cfRule type="containsText" dxfId="92" priority="61" operator="containsText" text="10">
       <formula>NOT(ISERROR(SEARCH("10",B8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:C14">
-    <cfRule type="containsText" dxfId="59" priority="60" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="91" priority="60" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",B12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="59" operator="containsText" text="2">
+    <cfRule type="containsText" dxfId="90" priority="59" operator="containsText" text="2">
       <formula>NOT(ISERROR(SEARCH("2",B12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="58" operator="containsText" text="3">
+    <cfRule type="containsText" dxfId="89" priority="58" operator="containsText" text="3">
       <formula>NOT(ISERROR(SEARCH("3",B12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="56" operator="containsText" text="5">
+    <cfRule type="containsText" dxfId="88" priority="56" operator="containsText" text="5">
       <formula>NOT(ISERROR(SEARCH("5",B12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="57" operator="containsText" text="4">
+    <cfRule type="containsText" dxfId="87" priority="57" operator="containsText" text="4">
       <formula>NOT(ISERROR(SEARCH("4",B12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="55" operator="containsText" text="6">
+    <cfRule type="containsText" dxfId="86" priority="55" operator="containsText" text="6">
       <formula>NOT(ISERROR(SEARCH("6",B12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="54" operator="containsText" text="7">
+    <cfRule type="containsText" dxfId="85" priority="54" operator="containsText" text="7">
       <formula>NOT(ISERROR(SEARCH("7",B12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="53" operator="containsText" text="8">
+    <cfRule type="containsText" dxfId="84" priority="53" operator="containsText" text="8">
       <formula>NOT(ISERROR(SEARCH("8",B12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="52" operator="containsText" text="9">
+    <cfRule type="containsText" dxfId="83" priority="52" operator="containsText" text="9">
       <formula>NOT(ISERROR(SEARCH("9",B12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="51" operator="containsText" text="10">
+    <cfRule type="containsText" dxfId="82" priority="51" operator="containsText" text="10">
       <formula>NOT(ISERROR(SEARCH("10",B12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:C19">
-    <cfRule type="containsText" dxfId="49" priority="41" operator="containsText" text="10">
+    <cfRule type="containsText" dxfId="81" priority="41" operator="containsText" text="10">
       <formula>NOT(ISERROR(SEARCH("10",B17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="42" operator="containsText" text="9">
+    <cfRule type="containsText" dxfId="80" priority="42" operator="containsText" text="9">
       <formula>NOT(ISERROR(SEARCH("9",B17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="43" operator="containsText" text="8">
+    <cfRule type="containsText" dxfId="79" priority="43" operator="containsText" text="8">
       <formula>NOT(ISERROR(SEARCH("8",B17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="44" operator="containsText" text="7">
+    <cfRule type="containsText" dxfId="78" priority="44" operator="containsText" text="7">
       <formula>NOT(ISERROR(SEARCH("7",B17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="45" operator="containsText" text="6">
+    <cfRule type="containsText" dxfId="77" priority="45" operator="containsText" text="6">
       <formula>NOT(ISERROR(SEARCH("6",B17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="46" operator="containsText" text="5">
+    <cfRule type="containsText" dxfId="76" priority="46" operator="containsText" text="5">
       <formula>NOT(ISERROR(SEARCH("5",B17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="47" operator="containsText" text="4">
+    <cfRule type="containsText" dxfId="75" priority="47" operator="containsText" text="4">
       <formula>NOT(ISERROR(SEARCH("4",B17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="48" operator="containsText" text="3">
+    <cfRule type="containsText" dxfId="74" priority="48" operator="containsText" text="3">
       <formula>NOT(ISERROR(SEARCH("3",B17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="49" operator="containsText" text="2">
+    <cfRule type="containsText" dxfId="73" priority="49" operator="containsText" text="2">
       <formula>NOT(ISERROR(SEARCH("2",B17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="50" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="72" priority="50" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",B17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:C24">
-    <cfRule type="containsText" dxfId="39" priority="38" operator="containsText" text="3">
+    <cfRule type="containsText" dxfId="71" priority="38" operator="containsText" text="3">
       <formula>NOT(ISERROR(SEARCH("3",B22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="40" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="70" priority="40" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",B22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="39" operator="containsText" text="2">
+    <cfRule type="containsText" dxfId="69" priority="39" operator="containsText" text="2">
       <formula>NOT(ISERROR(SEARCH("2",B22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="31" operator="containsText" text="10">
+    <cfRule type="containsText" dxfId="68" priority="31" operator="containsText" text="10">
       <formula>NOT(ISERROR(SEARCH("10",B22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="37" operator="containsText" text="4">
+    <cfRule type="containsText" dxfId="67" priority="37" operator="containsText" text="4">
       <formula>NOT(ISERROR(SEARCH("4",B22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="36" operator="containsText" text="5">
+    <cfRule type="containsText" dxfId="66" priority="36" operator="containsText" text="5">
       <formula>NOT(ISERROR(SEARCH("5",B22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="34" operator="containsText" text="7">
+    <cfRule type="containsText" dxfId="65" priority="34" operator="containsText" text="7">
       <formula>NOT(ISERROR(SEARCH("7",B22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="35" operator="containsText" text="6">
+    <cfRule type="containsText" dxfId="64" priority="35" operator="containsText" text="6">
       <formula>NOT(ISERROR(SEARCH("6",B22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="33" operator="containsText" text="8">
+    <cfRule type="containsText" dxfId="63" priority="33" operator="containsText" text="8">
       <formula>NOT(ISERROR(SEARCH("8",B22)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="32" operator="containsText" text="9">
+    <cfRule type="containsText" dxfId="62" priority="32" operator="containsText" text="9">
       <formula>NOT(ISERROR(SEARCH("9",B22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:C29">
-    <cfRule type="containsText" dxfId="29" priority="30" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="61" priority="30" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",B27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="2">
+    <cfRule type="containsText" dxfId="60" priority="29" operator="containsText" text="2">
       <formula>NOT(ISERROR(SEARCH("2",B27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="28" operator="containsText" text="3">
+    <cfRule type="containsText" dxfId="59" priority="28" operator="containsText" text="3">
       <formula>NOT(ISERROR(SEARCH("3",B27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="27" operator="containsText" text="4">
+    <cfRule type="containsText" dxfId="58" priority="27" operator="containsText" text="4">
       <formula>NOT(ISERROR(SEARCH("4",B27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="5">
+    <cfRule type="containsText" dxfId="57" priority="26" operator="containsText" text="5">
       <formula>NOT(ISERROR(SEARCH("5",B27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="23" operator="containsText" text="8">
+    <cfRule type="containsText" dxfId="56" priority="23" operator="containsText" text="8">
       <formula>NOT(ISERROR(SEARCH("8",B27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="6">
+    <cfRule type="containsText" dxfId="55" priority="25" operator="containsText" text="6">
       <formula>NOT(ISERROR(SEARCH("6",B27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="7">
+    <cfRule type="containsText" dxfId="54" priority="24" operator="containsText" text="7">
       <formula>NOT(ISERROR(SEARCH("7",B27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="9">
+    <cfRule type="containsText" dxfId="53" priority="22" operator="containsText" text="9">
       <formula>NOT(ISERROR(SEARCH("9",B27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="21" operator="containsText" text="10">
+    <cfRule type="containsText" dxfId="52" priority="21" operator="containsText" text="10">
       <formula>NOT(ISERROR(SEARCH("10",B27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32:C34">
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="4">
+    <cfRule type="containsText" dxfId="51" priority="17" operator="containsText" text="4">
       <formula>NOT(ISERROR(SEARCH("4",B32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="12" operator="containsText" text="9">
+    <cfRule type="containsText" dxfId="50" priority="12" operator="containsText" text="9">
       <formula>NOT(ISERROR(SEARCH("9",B32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="20" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="49" priority="20" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",B32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="19" operator="containsText" text="2">
+    <cfRule type="containsText" dxfId="48" priority="19" operator="containsText" text="2">
       <formula>NOT(ISERROR(SEARCH("2",B32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="3">
+    <cfRule type="containsText" dxfId="47" priority="18" operator="containsText" text="3">
       <formula>NOT(ISERROR(SEARCH("3",B32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="5">
+    <cfRule type="containsText" dxfId="46" priority="16" operator="containsText" text="5">
       <formula>NOT(ISERROR(SEARCH("5",B32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="6">
+    <cfRule type="containsText" dxfId="45" priority="15" operator="containsText" text="6">
       <formula>NOT(ISERROR(SEARCH("6",B32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="14" operator="containsText" text="7">
+    <cfRule type="containsText" dxfId="44" priority="14" operator="containsText" text="7">
       <formula>NOT(ISERROR(SEARCH("7",B32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="8">
+    <cfRule type="containsText" dxfId="43" priority="13" operator="containsText" text="8">
       <formula>NOT(ISERROR(SEARCH("8",B32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="10">
+    <cfRule type="containsText" dxfId="42" priority="11" operator="containsText" text="10">
       <formula>NOT(ISERROR(SEARCH("10",B32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37:C39">
-    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="9">
+    <cfRule type="containsText" dxfId="41" priority="2" operator="containsText" text="9">
       <formula>NOT(ISERROR(SEARCH("9",B37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="8">
+    <cfRule type="containsText" dxfId="40" priority="3" operator="containsText" text="8">
       <formula>NOT(ISERROR(SEARCH("8",B37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="7">
+    <cfRule type="containsText" dxfId="39" priority="4" operator="containsText" text="7">
       <formula>NOT(ISERROR(SEARCH("7",B37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="6">
+    <cfRule type="containsText" dxfId="38" priority="5" operator="containsText" text="6">
       <formula>NOT(ISERROR(SEARCH("6",B37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="5">
+    <cfRule type="containsText" dxfId="37" priority="6" operator="containsText" text="5">
       <formula>NOT(ISERROR(SEARCH("5",B37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="3">
+    <cfRule type="containsText" dxfId="36" priority="8" operator="containsText" text="3">
       <formula>NOT(ISERROR(SEARCH("3",B37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="9" operator="containsText" text="2">
+    <cfRule type="containsText" dxfId="35" priority="9" operator="containsText" text="2">
       <formula>NOT(ISERROR(SEARCH("2",B37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="10" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="34" priority="10" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",B37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="7" operator="containsText" text="4">
+    <cfRule type="containsText" dxfId="33" priority="7" operator="containsText" text="4">
       <formula>NOT(ISERROR(SEARCH("4",B37)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="10">
+    <cfRule type="containsText" dxfId="32" priority="1" operator="containsText" text="10">
       <formula>NOT(ISERROR(SEARCH("10",B37)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>